<commit_message>
feat: add cyfun small self assessment
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun-small-self-assessment.xlsx
+++ b/tools/excel/ccb/cyfun-small-self-assessment.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF174F12-6833-4B40-BBFF-0E270E24CB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5D3B9-5661-414A-81FC-249CE5CA5EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{09EDE502-9E78-CA46-8718-A2BE9763EDA0}"/>
+    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{09EDE502-9E78-CA46-8718-A2BE9763EDA0}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
     <sheet name="requirements" sheetId="2" r:id="rId2"/>
     <sheet name="scores" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">requirements!$A$1:$E$9</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AF4AC7-EE1A-3A47-9EE9-901F2B2BC0CE}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="207" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6400D6E-455F-F24F-B7F9-61690E28E6B4}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1073,12 +1076,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1086,21 +1098,33 @@
         <v>96</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1108,21 +1132,33 @@
         <v>96</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1130,21 +1166,33 @@
         <v>96</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1152,105 +1200,22 @@
         <v>96</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="7" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E9" xr:uid="{D6400D6E-455F-F24F-B7F9-61690E28E6B4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>